<commit_message>
Ajout Fin ASP.NET Semaine 4
</commit_message>
<xml_diff>
--- a/I314B_ASP.NET/Semaine 3.4 - SportsStore Roadmap.xlsx
+++ b/I314B_ASP.NET/Semaine 3.4 - SportsStore Roadmap.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -76,7 +76,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +113,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -120,8 +127,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="20"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -210,56 +224,51 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -435,31 +444,31 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -898,56 +907,57 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.125" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.25" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.125" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="13"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="12"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="9" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="10">
@@ -957,22 +967,22 @@
         <f>D3</f>
         <v>2</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="9">
         <v>3</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="12">
         <f>+F3</f>
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="A4" s="7">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="8"/>
+      <c r="C4" s="9"/>
       <c r="D4" s="10">
         <v>2</v>
       </c>
@@ -980,20 +990,22 @@
         <f t="shared" ref="E4:E12" si="0">E3+D4</f>
         <v>4</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="7">
+      <c r="F4" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="G4" s="12">
         <f t="shared" ref="G4:G6" si="1">G3+F4</f>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="8"/>
+      <c r="C5" s="9"/>
       <c r="D5" s="10">
         <v>2</v>
       </c>
@@ -1001,20 +1013,20 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="7">
+      <c r="F5" s="9"/>
+      <c r="G5" s="12">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="7">
         <v>4</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" s="9"/>
       <c r="D6" s="10">
         <v>2</v>
       </c>
@@ -1022,20 +1034,20 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="7">
+      <c r="F6" s="9"/>
+      <c r="G6" s="12">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="A7" s="7">
         <v>5</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="9"/>
       <c r="D7" s="10">
         <v>2</v>
       </c>
@@ -1043,20 +1055,20 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="7">
+      <c r="F7" s="9"/>
+      <c r="G7" s="12">
         <f>G6+F7</f>
-        <v>3</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="A8" s="7">
         <v>6</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="8"/>
+      <c r="C8" s="9"/>
       <c r="D8" s="10">
         <v>2</v>
       </c>
@@ -1064,20 +1076,20 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="7">
+      <c r="F8" s="9"/>
+      <c r="G8" s="12">
         <f t="shared" ref="G8:G12" si="2">G7+F8</f>
-        <v>3</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="A9" s="7">
         <v>7</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="8"/>
+      <c r="C9" s="9"/>
       <c r="D9" s="10">
         <v>2</v>
       </c>
@@ -1085,20 +1097,20 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="7">
+      <c r="F9" s="9"/>
+      <c r="G9" s="12">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+      <c r="A10" s="7">
         <v>8</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="8"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="10">
         <v>2</v>
       </c>
@@ -1106,20 +1118,20 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="7">
+      <c r="F10" s="9"/>
+      <c r="G10" s="12">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+      <c r="A11" s="7">
         <v>9</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="8"/>
+      <c r="C11" s="9"/>
       <c r="D11" s="10">
         <v>2</v>
       </c>
@@ -1127,20 +1139,20 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="7">
+      <c r="F11" s="9"/>
+      <c r="G11" s="12">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="A12" s="7">
         <v>10</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="8"/>
+      <c r="C12" s="9"/>
       <c r="D12" s="10">
         <v>2</v>
       </c>
@@ -1148,101 +1160,101 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="7">
+      <c r="F12" s="9"/>
+      <c r="G12" s="12">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="2"/>
+      <c r="C13" s="13"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="2"/>
+      <c r="C14" s="13"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C15" s="2"/>
+      <c r="C15" s="13"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="2"/>
+      <c r="C16" s="13"/>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="2"/>
+      <c r="C17" s="13"/>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="2"/>
+      <c r="C18" s="13"/>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="2"/>
+      <c r="C19" s="13"/>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="2"/>
+      <c r="C20" s="13"/>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="2"/>
+      <c r="C21" s="13"/>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" s="2"/>
+      <c r="C22" s="13"/>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23" s="2"/>
+      <c r="C23" s="13"/>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C24" s="2"/>
+      <c r="C24" s="13"/>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C25" s="2"/>
+      <c r="C25" s="13"/>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C26" s="2"/>
+      <c r="C26" s="13"/>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C27" s="2"/>
+      <c r="C27" s="13"/>
     </row>
     <row r="28" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C28" s="2"/>
+      <c r="C28" s="13"/>
     </row>
     <row r="29" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C29" s="2"/>
+      <c r="C29" s="13"/>
     </row>
     <row r="30" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C30" s="2"/>
+      <c r="C30" s="13"/>
     </row>
     <row r="31" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C31" s="2"/>
+      <c r="C31" s="13"/>
     </row>
     <row r="32" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C32" s="2"/>
+      <c r="C32" s="13"/>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33" s="2"/>
+      <c r="C33" s="13"/>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C34" s="2"/>
+      <c r="C34" s="13"/>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C35" s="2"/>
+      <c r="C35" s="13"/>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C36" s="2"/>
+      <c r="C36" s="13"/>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C37" s="2"/>
+      <c r="C37" s="13"/>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C38" s="2"/>
+      <c r="C38" s="13"/>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C39" s="2"/>
+      <c r="C39" s="13"/>
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C40" s="2"/>
+      <c r="C40" s="13"/>
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C41" s="2"/>
+      <c r="C41" s="13"/>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C42" s="2"/>
+      <c r="C42" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>